<commit_message>
makes changes to codebook
</commit_message>
<xml_diff>
--- a/data/nfl_codebook.xlsx
+++ b/data/nfl_codebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonleff/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonleff/Library/Containers/com.microsoft.Excel/Data/Desktop/math456/project/456nflproject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1937DD1E-F69E-4741-9BAC-9E6808011734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71D42CA-0C97-D649-8A22-AFC5CEF55458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{E43AF12B-0E02-A24C-968C-D8F1BD07D68E}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{E43AF12B-0E02-A24C-968C-D8F1BD07D68E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +396,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339C334E-470F-1E4C-9E56-069E54512E1F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
jenny was here hehe
</commit_message>
<xml_diff>
--- a/data/nfl_codebook.xlsx
+++ b/data/nfl_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonleff/Library/Containers/com.microsoft.Excel/Data/Desktop/math456/project/456nflproject/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennytran/nflproject2/nflproject456/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71D42CA-0C97-D649-8A22-AFC5CEF55458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5144FA5D-2C7C-A744-A0B0-A8449A66110C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{E43AF12B-0E02-A24C-968C-D8F1BD07D68E}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{E43AF12B-0E02-A24C-968C-D8F1BD07D68E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Data Type</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339C334E-470F-1E4C-9E56-069E54512E1F}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,6 +421,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>